<commit_message>
Included paper demo Excel sheet.
</commit_message>
<xml_diff>
--- a/paper_demo.xlsx
+++ b/paper_demo.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14240" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13940" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="notes" sheetId="1" r:id="rId1"/>
+    <sheet name="v2.5" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Paper</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,6 +68,45 @@
   <si>
     <t>Dimensionality</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>Figure 1</t>
+  </si>
+  <si>
+    <t>Figure 2</t>
+  </si>
+  <si>
+    <t>Figure 3</t>
+  </si>
+  <si>
+    <t>Figure 4</t>
+  </si>
+  <si>
+    <t>Figure 5</t>
+  </si>
+  <si>
+    <t>Figure 6</t>
+  </si>
+  <si>
+    <t>Figure 7</t>
+  </si>
+  <si>
+    <t>Figure 8</t>
+  </si>
+  <si>
+    <t>Figure 9</t>
+  </si>
+  <si>
+    <t>Figure 10</t>
+  </si>
+  <si>
+    <t>demo3D27</t>
+  </si>
+  <si>
+    <t>Johnson et a. (2105)</t>
   </si>
 </sst>
 </file>
@@ -77,14 +117,14 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -93,7 +133,7 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -102,7 +142,7 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -149,11 +189,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="普通" xfId="0" builtinId="0"/>
-    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -484,7 +524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -693,7 +733,72 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
added demos corresponding to last 10 CO published papers to paper_demos.xlsx
</commit_message>
<xml_diff>
--- a/paper_demo.xlsx
+++ b/paper_demo.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13940" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Paper</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -107,6 +107,72 @@
   </si>
   <si>
     <t>Johnson et a. (2105)</t>
+  </si>
+  <si>
+    <t>Li et al. (2012)</t>
+  </si>
+  <si>
+    <t>Buck et al. (2012)</t>
+  </si>
+  <si>
+    <t>Murphy (2012)</t>
+  </si>
+  <si>
+    <t>Peng and Murphy (2011)</t>
+  </si>
+  <si>
+    <t>Shariff et al (2011)</t>
+  </si>
+  <si>
+    <t>Murphy (2010)</t>
+  </si>
+  <si>
+    <t>Shariff et al. (2010)</t>
+  </si>
+  <si>
+    <t>Peng et al. (2009)</t>
+  </si>
+  <si>
+    <t>Rohde et al. (2008)</t>
+  </si>
+  <si>
+    <t>demo3D04</t>
+  </si>
+  <si>
+    <t>demo3D00, demo3D02</t>
+  </si>
+  <si>
+    <t>demo3Dimg2microtubule_model</t>
+  </si>
+  <si>
+    <t>demo2D01</t>
+  </si>
+  <si>
+    <t>demo3D11</t>
+  </si>
+  <si>
+    <t>demo2D02, demo3D09</t>
+  </si>
+  <si>
+    <t>demo3D02</t>
+  </si>
+  <si>
+    <t>demo3D01</t>
+  </si>
+  <si>
+    <t>demo2D00</t>
+  </si>
+  <si>
+    <t>demo3D01, demo3D14</t>
+  </si>
+  <si>
+    <t>demo3D07, demo3D06</t>
+  </si>
+  <si>
+    <t>demo2D04, demo3D15, demo3D20</t>
+  </si>
+  <si>
+    <t>demo3D15</t>
   </si>
 </sst>
 </file>
@@ -119,7 +185,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -176,8 +241,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -188,11 +257,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -743,10 +816,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -797,8 +870,120 @@
         <v>24</v>
       </c>
     </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Renamed demo3Dimg2microtubule_model to demo3D35.
</commit_message>
<xml_diff>
--- a/paper_demo.xlsx
+++ b/paper_demo.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12800" windowHeight="15460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="1" r:id="rId1"/>
@@ -142,9 +142,6 @@
     <t>demo3D00, demo3D02</t>
   </si>
   <si>
-    <t>demo3Dimg2microtubule_model</t>
-  </si>
-  <si>
     <t>demo2D01</t>
   </si>
   <si>
@@ -173,6 +170,9 @@
   </si>
   <si>
     <t>demo3D15</t>
+  </si>
+  <si>
+    <t>demo3D35</t>
   </si>
 </sst>
 </file>
@@ -819,7 +819,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -881,7 +881,7 @@
         <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -889,13 +889,13 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>39</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
       </c>
       <c r="G4" t="s">
         <v>35</v>
@@ -906,10 +906,10 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="s">
         <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -917,10 +917,10 @@
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -939,10 +939,10 @@
         <v>31</v>
       </c>
       <c r="E8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
         <v>42</v>
-      </c>
-      <c r="G8" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -950,19 +950,19 @@
         <v>32</v>
       </c>
       <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" t="s">
         <v>44</v>
       </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="I9" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -970,10 +970,10 @@
         <v>33</v>
       </c>
       <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" t="s">
         <v>46</v>
-      </c>
-      <c r="F10" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -983,7 +983,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Removed empty line from sheet.
</commit_message>
<xml_diff>
--- a/paper_demo.xlsx
+++ b/paper_demo.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26606"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/icaoberg/code/cellorganizer-docs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="1" r:id="rId1"/>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>Paper</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -131,9 +136,6 @@
   </si>
   <si>
     <t>Peng et al. (2009)</t>
-  </si>
-  <si>
-    <t>Rohde et al. (2008)</t>
   </si>
   <si>
     <t>demo3D04</t>
@@ -270,6 +272,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -601,12 +608,12 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -626,7 +633,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>201</v>
       </c>
@@ -638,7 +645,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>201</v>
       </c>
@@ -648,7 +655,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>201</v>
       </c>
@@ -658,7 +665,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>201</v>
       </c>
@@ -668,7 +675,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>201</v>
       </c>
@@ -678,7 +685,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>201</v>
       </c>
@@ -688,7 +695,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>201</v>
       </c>
@@ -698,7 +705,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>202</v>
       </c>
@@ -708,7 +715,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>202</v>
       </c>
@@ -718,7 +725,7 @@
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>202</v>
       </c>
@@ -728,7 +735,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>202</v>
       </c>
@@ -738,7 +745,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>203</v>
       </c>
@@ -749,7 +756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>204</v>
       </c>
@@ -760,7 +767,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>204</v>
       </c>
@@ -771,7 +778,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>201</v>
       </c>
@@ -779,7 +786,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>202</v>
       </c>
@@ -787,7 +794,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>203</v>
       </c>
@@ -795,7 +802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>204</v>
       </c>
@@ -806,28 +813,23 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -862,7 +864,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -870,123 +872,113 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
       <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" t="s">
-        <v>39</v>
-      </c>
       <c r="G4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>28</v>
       </c>
       <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>31</v>
       </c>
       <c r="E8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
         <v>41</v>
       </c>
-      <c r="G8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>32</v>
       </c>
       <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
         <v>43</v>
       </c>
-      <c r="E9" t="s">
-        <v>44</v>
-      </c>
       <c r="G9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>33</v>
       </c>
       <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" t="s">
         <v>45</v>
-      </c>
-      <c r="F10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>